<commit_message>
Add title, bestseller to specs, revamp structure to conform to the tutors' guidelines
</commit_message>
<xml_diff>
--- a/csv/sources/book.xlsx
+++ b/csv/sources/book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casa\Desktop\hyp-project\csv\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECE1D4C-A784-43D3-977C-5EFDE15B194A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CD5D96-0901-4B2A-BA8A-9BD0357C37EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3220" yWindow="2120" windowWidth="8100" windowHeight="7360" xr2:uid="{4E3BCF33-7C41-4632-85A3-F999C8980790}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4E3BCF33-7C41-4632-85A3-F999C8980790}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="181">
   <si>
     <t>book_id</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>A Criminal Defense</t>
-  </si>
-  <si>
-    <t>An Engineered Justice</t>
   </si>
   <si>
     <t>The River</t>
@@ -431,9 +428,6 @@
     <t>for_esme_with_love_and_squalor.jpeg</t>
   </si>
   <si>
-    <t>chronicles_of_a_radical_hag_with_recipes_a_novel.jpeg</t>
-  </si>
-  <si>
     <t>east_of_eden.jpeg</t>
   </si>
   <si>
@@ -470,9 +464,6 @@
     <t>a_criminal_defense.jpeg</t>
   </si>
   <si>
-    <t>an_engineered_justice.jpeg</t>
-  </si>
-  <si>
     <t>the_river.jpeg</t>
   </si>
   <si>
@@ -527,9 +518,6 @@
     <t>war</t>
   </si>
   <si>
-    <t>horror</t>
-  </si>
-  <si>
     <t>love</t>
   </si>
   <si>
@@ -579,6 +567,21 @@
   </si>
   <si>
     <t>non fiction</t>
+  </si>
+  <si>
+    <t>An Engineered Injustice</t>
+  </si>
+  <si>
+    <t>an_engineered_injustice.jpeg</t>
+  </si>
+  <si>
+    <t>chronicles_of_a_radical_hag.jpeg</t>
+  </si>
+  <si>
+    <t>fear</t>
+  </si>
+  <si>
+    <t>is_bestseller</t>
   </si>
 </sst>
 </file>
@@ -588,7 +591,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,6 +621,14 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -674,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -707,6 +718,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1021,12 +1033,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3D2FCB-0BDA-4308-8A96-936223DF5329}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1034,10 +1046,10 @@
     <col min="1" max="1" width="20.6328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="23.26953125" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" style="2"/>
-    <col min="7" max="7" width="15.81640625" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1057,19 +1069,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>8893517140</v>
       </c>
@@ -1077,31 +1092,34 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="6">
+        <v>41309</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" s="6">
-        <v>41309</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>165</v>
-      </c>
       <c r="J2" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>8893517141</v>
       </c>
@@ -1109,31 +1127,34 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" s="5">
+        <v>41310</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G3" s="5">
-        <v>41310</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>8893517142</v>
       </c>
@@ -1141,31 +1162,34 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" s="5">
+        <v>41311</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G4" s="5">
-        <v>41311</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J4" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>8893517143</v>
       </c>
@@ -1173,63 +1197,69 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" s="5">
+        <v>36929</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G5" s="5">
-        <v>36929</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J5" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>8893517144</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H6" s="5">
+        <v>41313</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G6" s="5">
-        <v>41313</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J6" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>8893517145</v>
       </c>
@@ -1237,31 +1267,34 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="5">
+        <v>39487</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G7" s="5">
-        <v>39487</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J7" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>8893517146</v>
       </c>
@@ -1269,63 +1302,69 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H8" s="5">
+        <v>41315</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G8" s="5">
-        <v>41315</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J8" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>8893517147</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="5">
+        <v>41316</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G9" s="5">
-        <v>41316</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J9" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>8893517148</v>
       </c>
@@ -1333,63 +1372,69 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="5">
+        <v>41317</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G10" s="5">
-        <v>41317</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J10" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>8893517149</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H11" s="5">
+        <v>38396</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G11" s="5">
-        <v>38396</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J11" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>8893517150</v>
       </c>
@@ -1397,31 +1442,34 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H12" s="5">
+        <v>41319</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G12" s="5">
-        <v>41319</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J12" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>8893517151</v>
       </c>
@@ -1429,31 +1477,35 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G13" s="5">
+        <v>149</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="5">
         <v>41320</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="I13" s="3" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>8893517152</v>
       </c>
@@ -1461,31 +1513,34 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H14" s="5">
+        <v>40955</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G14" s="5">
-        <v>40955</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J14" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>8893517153</v>
       </c>
@@ -1493,31 +1548,34 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" s="5">
+        <v>41322</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G15" s="5">
-        <v>41322</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J15" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K15" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>8893517154</v>
       </c>
@@ -1525,31 +1583,34 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H16" s="5">
+        <v>41688</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="G16" s="5">
-        <v>41688</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J16" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K16" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>8893517156</v>
       </c>
@@ -1557,31 +1618,34 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="5">
+        <v>42054</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G17" s="5">
-        <v>42054</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J17" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>8893517158</v>
       </c>
@@ -1589,31 +1653,34 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" s="5">
+        <v>42420</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G18" s="5">
-        <v>42420</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J18" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K18" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>8893517159</v>
       </c>
@@ -1621,31 +1688,34 @@
         <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G19" s="5">
+        <v>148</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H19" s="5">
         <v>41326</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="I19" s="3" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>8893517160</v>
       </c>
@@ -1653,31 +1723,34 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="5">
+        <v>39135</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G20" s="5">
-        <v>39135</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J20" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>8893517162</v>
       </c>
@@ -1685,31 +1758,34 @@
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G21" s="5">
+        <v>149</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" s="5">
         <v>41328</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I21" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>8893517163</v>
       </c>
@@ -1717,31 +1793,34 @@
         <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H22" s="5">
+        <v>41329</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G22" s="5">
-        <v>41329</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J22" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>8893517164</v>
       </c>
@@ -1749,31 +1828,34 @@
         <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G23" s="5">
+        <v>149</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H23" s="5">
         <v>41330</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I23" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>8893517165</v>
       </c>
@@ -1781,31 +1863,34 @@
         <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G24" s="5">
+        <v>149</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H24" s="5">
         <v>41331</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I24" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>8893517166</v>
       </c>
@@ -1813,31 +1898,34 @@
         <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G25" s="5">
+        <v>149</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H25" s="5">
         <v>41332</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I25" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <v>8893517167</v>
       </c>
@@ -1845,31 +1933,34 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H26" s="5">
+        <v>41333</v>
+      </c>
+      <c r="I26" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G26" s="5">
-        <v>41333</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="J26" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>8893517168</v>
       </c>
@@ -1877,31 +1968,34 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G27" s="5">
+        <v>149</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H27" s="5">
         <v>41334</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I27" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>8893517169</v>
       </c>
@@ -1909,31 +2003,34 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G28" s="5">
+        <v>149</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H28" s="5">
         <v>35126</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I28" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>8893517170</v>
       </c>
@@ -1941,31 +2038,34 @@
         <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G29" s="5">
+        <v>149</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H29" s="5">
         <v>37683</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I29" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <v>8893517171</v>
       </c>
@@ -1973,31 +2073,34 @@
         <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G30" s="5">
+        <v>149</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H30" s="5">
         <v>41337</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I30" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>8893517172</v>
       </c>
@@ -2005,31 +2108,34 @@
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G31" s="5">
+        <v>149</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H31" s="5">
         <v>43164</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I31" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <v>8893517173</v>
       </c>
@@ -2037,31 +2143,34 @@
         <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G32" s="5">
+        <v>149</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H32" s="5">
         <v>41339</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I32" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>8893517174</v>
       </c>
@@ -2069,31 +2178,34 @@
         <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G33" s="5">
+        <v>149</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H33" s="5">
         <v>41340</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I33" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
         <v>8893517175</v>
       </c>
@@ -2101,31 +2213,34 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G34" s="5">
+        <v>148</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H34" s="5">
         <v>43532</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I34" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <v>8893517176</v>
       </c>
@@ -2133,31 +2248,34 @@
         <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G35" s="5">
+        <v>149</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H35" s="5">
         <v>41342</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I35" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <v>8893517177</v>
       </c>
@@ -2165,31 +2283,34 @@
         <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G36" s="5">
+        <v>149</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H36" s="5">
         <v>41343</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="I36" s="3" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <v>8893517178</v>
       </c>
@@ -2197,31 +2318,34 @@
         <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G37" s="5">
+        <v>149</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H37" s="5">
         <v>41344</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I37" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <v>8893517179</v>
       </c>
@@ -2229,31 +2353,34 @@
         <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G38" s="5">
+        <v>148</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H38" s="5">
         <v>32944</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I38" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <v>8893517180</v>
       </c>
@@ -2261,31 +2388,34 @@
         <v>44</v>
       </c>
       <c r="C39" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G39" s="5">
+        <v>149</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H39" s="5">
         <v>41346</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="I39" s="3" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
         <v>8893517181</v>
       </c>
@@ -2293,63 +2423,69 @@
         <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G40" s="5">
+        <v>149</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H40" s="5">
         <v>41347</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="I40" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1">
         <v>8893517182</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G41" s="5">
+        <v>149</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H41" s="5">
         <v>25642</v>
       </c>
-      <c r="H41" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>165</v>
+      <c r="I41" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="1">
         <v>8893517183</v>
       </c>
@@ -2357,351 +2493,384 @@
         <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G42" s="5">
+        <v>149</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H42" s="5">
         <v>32218</v>
       </c>
-      <c r="H42" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>165</v>
+      <c r="I42" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
         <v>8893517184</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>47</v>
+        <v>176</v>
       </c>
       <c r="C43" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G43" s="5">
+        <v>149</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H43" s="5">
         <v>41350</v>
       </c>
-      <c r="H43" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>165</v>
+      <c r="I43" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
         <v>8893517185</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G44" s="5">
+        <v>149</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H44" s="5">
         <v>41351</v>
       </c>
-      <c r="H44" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>165</v>
+      <c r="I44" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <v>8893517186</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G45" s="5">
+        <v>149</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H45" s="5">
         <v>31125</v>
       </c>
-      <c r="H45" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>165</v>
+      <c r="I45" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <v>8893517187</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G46" s="5">
+        <v>148</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H46" s="5">
         <v>41353</v>
       </c>
-      <c r="H46" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>165</v>
+      <c r="I46" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <v>8893517188</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G47" s="5">
+        <v>149</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H47" s="5">
         <v>34049</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="I47" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K47" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I47" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
         <v>8893517189</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G48" s="5">
+      <c r="H48" s="5">
         <v>24553</v>
       </c>
-      <c r="H48" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>165</v>
+      <c r="I48" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <v>8893517190</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G49" s="5">
+        <v>149</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H49" s="5">
         <v>41356</v>
       </c>
-      <c r="H49" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>165</v>
+      <c r="I49" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="10">
         <v>8893517191</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C50" t="s">
+        <v>168</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="D50" s="12" t="s">
-        <v>176</v>
-      </c>
       <c r="E50" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G50" s="5">
+        <v>148</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H50" s="5">
         <v>43241</v>
       </c>
-      <c r="H50" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="I50" s="3" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="10">
         <v>8893517192</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C51" t="s">
+        <v>170</v>
+      </c>
+      <c r="D51" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="C51" t="s">
-        <v>174</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>177</v>
-      </c>
       <c r="E51" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G51" s="5">
+        <v>148</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H51" s="5">
         <v>43622</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="I51" s="3" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="10">
         <v>8893517193</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C52" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G52" s="5">
+        <v>148</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H52" s="5">
         <v>43625</v>
       </c>
-      <c r="H52" s="4" t="s">
+      <c r="I52" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K52" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I52" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D60" s="1"/>
     </row>
   </sheetData>

</xml_diff>